<commit_message>
aynonyms parsing is updated
</commit_message>
<xml_diff>
--- a/Results/Falmec/syn_report_housedorf.xlsx
+++ b/Results/Falmec/syn_report_housedorf.xlsx
@@ -990,8 +990,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:C227"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="C121" sqref="C121"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C104" sqref="C104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1011,7 +1011,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" hidden="1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1019,7 +1019,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" hidden="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1027,7 +1027,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" hidden="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1035,7 +1035,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" hidden="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1043,7 +1043,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" hidden="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1051,7 +1051,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" hidden="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1059,7 +1059,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" hidden="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1067,7 +1067,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" hidden="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1075,7 +1075,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:3" hidden="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1083,7 +1083,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:3" hidden="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1091,7 +1091,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:3" hidden="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -1099,18 +1099,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:3" hidden="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>15</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>
       </c>
-      <c r="C13">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" hidden="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -1118,7 +1115,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:3" hidden="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -1126,7 +1123,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:3" hidden="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -1134,7 +1131,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -1142,7 +1139,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -1150,7 +1147,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -1158,7 +1155,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -1166,7 +1163,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -1174,7 +1171,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -1182,7 +1179,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -1190,7 +1187,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -1198,7 +1195,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -1206,7 +1203,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -1214,7 +1211,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -1222,7 +1219,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>29</v>
       </c>
@@ -1230,7 +1227,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>30</v>
       </c>
@@ -1238,7 +1235,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>31</v>
       </c>
@@ -1246,7 +1243,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>32</v>
       </c>
@@ -1254,7 +1251,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>33</v>
       </c>
@@ -1262,7 +1259,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>34</v>
       </c>
@@ -1270,7 +1267,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>35</v>
       </c>
@@ -1278,7 +1275,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>36</v>
       </c>
@@ -1286,7 +1283,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -1294,7 +1291,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -1302,7 +1299,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -1310,7 +1307,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>36</v>
       </c>
@@ -1318,7 +1315,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>36</v>
       </c>
@@ -1326,7 +1323,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>36</v>
       </c>
@@ -1334,7 +1331,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>36</v>
       </c>
@@ -1342,7 +1339,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>36</v>
       </c>
@@ -1350,7 +1347,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>36</v>
       </c>
@@ -1358,7 +1355,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>36</v>
       </c>
@@ -1366,7 +1363,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>36</v>
       </c>
@@ -1374,7 +1371,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>36</v>
       </c>
@@ -1382,7 +1379,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>37</v>
       </c>
@@ -1390,7 +1387,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>38</v>
       </c>
@@ -1398,7 +1395,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>39</v>
       </c>
@@ -1406,7 +1403,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>40</v>
       </c>
@@ -1414,7 +1411,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>41</v>
       </c>
@@ -1422,7 +1419,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>42</v>
       </c>
@@ -1430,7 +1427,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>43</v>
       </c>
@@ -1438,7 +1435,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>44</v>
       </c>
@@ -1446,7 +1443,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>45</v>
       </c>
@@ -1454,7 +1451,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>46</v>
       </c>
@@ -1462,7 +1459,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>47</v>
       </c>
@@ -1470,7 +1467,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>48</v>
       </c>
@@ -1478,7 +1475,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
         <v>49</v>
       </c>
@@ -1486,7 +1483,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>50</v>
       </c>
@@ -1494,7 +1491,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
         <v>51</v>
       </c>
@@ -1502,7 +1499,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
         <v>52</v>
       </c>
@@ -1510,7 +1507,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
         <v>52</v>
       </c>
@@ -1518,7 +1515,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>53</v>
       </c>
@@ -1526,7 +1523,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
         <v>53</v>
       </c>
@@ -1534,7 +1531,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
         <v>54</v>
       </c>
@@ -1542,7 +1539,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>55</v>
       </c>
@@ -1550,7 +1547,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>56</v>
       </c>
@@ -1558,7 +1555,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>57</v>
       </c>
@@ -1566,7 +1563,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
         <v>58</v>
       </c>
@@ -1574,7 +1571,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
         <v>59</v>
       </c>
@@ -1582,7 +1579,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
         <v>60</v>
       </c>
@@ -1590,7 +1587,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
         <v>60</v>
       </c>
@@ -1598,7 +1595,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
         <v>61</v>
       </c>
@@ -1606,7 +1603,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
         <v>62</v>
       </c>
@@ -1614,7 +1611,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
         <v>63</v>
       </c>
@@ -1622,7 +1619,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
         <v>64</v>
       </c>
@@ -1630,7 +1627,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
         <v>64</v>
       </c>
@@ -1638,7 +1635,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
         <v>65</v>
       </c>
@@ -1646,7 +1643,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
         <v>65</v>
       </c>
@@ -1654,7 +1651,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
         <v>66</v>
       </c>
@@ -1662,7 +1659,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="83" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
         <v>67</v>
       </c>
@@ -1670,7 +1667,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="84" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
         <v>68</v>
       </c>
@@ -1678,7 +1675,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="85" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
         <v>69</v>
       </c>
@@ -1686,7 +1683,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="86" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
         <v>69</v>
       </c>
@@ -1694,7 +1691,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="87" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
         <v>70</v>
       </c>
@@ -1702,7 +1699,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="88" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
         <v>71</v>
       </c>
@@ -1710,7 +1707,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
         <v>72</v>
       </c>
@@ -1718,7 +1715,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
         <v>73</v>
       </c>
@@ -1726,7 +1723,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
         <v>74</v>
       </c>
@@ -1734,7 +1731,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
         <v>75</v>
       </c>
@@ -1742,7 +1739,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
         <v>76</v>
       </c>
@@ -1750,7 +1747,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
         <v>77</v>
       </c>
@@ -1758,7 +1755,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
         <v>78</v>
       </c>
@@ -1766,7 +1763,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
         <v>79</v>
       </c>
@@ -1774,7 +1771,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:3" hidden="1" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
         <v>80</v>
       </c>
@@ -1782,7 +1779,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:3" hidden="1" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
         <v>81</v>
       </c>
@@ -1790,7 +1787,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:3" hidden="1" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
         <v>82</v>
       </c>
@@ -1798,7 +1795,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:3" hidden="1" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
         <v>83</v>
       </c>
@@ -1806,7 +1803,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:3" hidden="1" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
         <v>84</v>
       </c>
@@ -1814,7 +1811,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:3" hidden="1" x14ac:dyDescent="0.45">
       <c r="A102" t="s">
         <v>84</v>
       </c>
@@ -1822,15 +1819,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="103" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A103" t="s">
         <v>85</v>
       </c>
       <c r="B103" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="104" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+      <c r="C103">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A104" t="s">
         <v>85</v>
       </c>
@@ -1838,7 +1838,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:3" hidden="1" x14ac:dyDescent="0.45">
       <c r="A105" t="s">
         <v>86</v>
       </c>
@@ -1846,7 +1846,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:3" hidden="1" x14ac:dyDescent="0.45">
       <c r="A106" t="s">
         <v>87</v>
       </c>
@@ -1854,7 +1854,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="107" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A107" t="s">
         <v>88</v>
       </c>
@@ -1862,7 +1862,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:3" hidden="1" x14ac:dyDescent="0.45">
       <c r="A108" t="s">
         <v>89</v>
       </c>
@@ -1870,7 +1870,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:3" hidden="1" x14ac:dyDescent="0.45">
       <c r="A109" t="s">
         <v>90</v>
       </c>
@@ -1878,7 +1878,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:3" hidden="1" x14ac:dyDescent="0.45">
       <c r="A110" t="s">
         <v>91</v>
       </c>
@@ -1886,7 +1886,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:3" hidden="1" x14ac:dyDescent="0.45">
       <c r="A111" t="s">
         <v>92</v>
       </c>
@@ -1894,7 +1894,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:3" hidden="1" x14ac:dyDescent="0.45">
       <c r="A112" t="s">
         <v>93</v>
       </c>
@@ -1902,7 +1902,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:3" hidden="1" x14ac:dyDescent="0.45">
       <c r="A113" t="s">
         <v>94</v>
       </c>
@@ -1910,7 +1910,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:3" hidden="1" x14ac:dyDescent="0.45">
       <c r="A114" t="s">
         <v>95</v>
       </c>
@@ -1918,7 +1918,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="115" spans="1:3" hidden="1" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A115" t="s">
         <v>96</v>
       </c>
@@ -1926,7 +1926,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="116" spans="1:3" hidden="1" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A116" t="s">
         <v>97</v>
       </c>
@@ -1934,7 +1934,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:3" hidden="1" x14ac:dyDescent="0.45">
       <c r="A117" t="s">
         <v>98</v>
       </c>
@@ -1942,7 +1942,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:3" hidden="1" x14ac:dyDescent="0.45">
       <c r="A118" t="s">
         <v>99</v>
       </c>
@@ -1950,7 +1950,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:3" hidden="1" x14ac:dyDescent="0.45">
       <c r="A119" t="s">
         <v>100</v>
       </c>
@@ -1958,18 +1958,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:3" hidden="1" x14ac:dyDescent="0.45">
       <c r="A120" t="s">
         <v>101</v>
       </c>
       <c r="B120" t="s">
         <v>4</v>
       </c>
-      <c r="C120">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.45">
+    </row>
+    <row r="121" spans="1:3" hidden="1" x14ac:dyDescent="0.45">
       <c r="A121" t="s">
         <v>101</v>
       </c>
@@ -1977,15 +1974,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:3" hidden="1" x14ac:dyDescent="0.45">
       <c r="A122" t="s">
         <v>102</v>
       </c>
       <c r="B122" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="C122">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" hidden="1" x14ac:dyDescent="0.45">
       <c r="A123" t="s">
         <v>102</v>
       </c>
@@ -1993,7 +1993,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:3" hidden="1" x14ac:dyDescent="0.45">
       <c r="A124" t="s">
         <v>103</v>
       </c>
@@ -2001,7 +2001,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:3" hidden="1" x14ac:dyDescent="0.45">
       <c r="A125" t="s">
         <v>104</v>
       </c>
@@ -2009,23 +2009,29 @@
         <v>4</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:3" hidden="1" x14ac:dyDescent="0.45">
       <c r="A126" t="s">
         <v>105</v>
       </c>
       <c r="B126" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="C126">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" hidden="1" x14ac:dyDescent="0.45">
       <c r="A127" t="s">
         <v>106</v>
       </c>
       <c r="B127" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="C127">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" hidden="1" x14ac:dyDescent="0.45">
       <c r="A128" t="s">
         <v>107</v>
       </c>
@@ -2033,7 +2039,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A129" t="s">
         <v>108</v>
       </c>
@@ -2041,7 +2047,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A130" t="s">
         <v>108</v>
       </c>
@@ -2049,7 +2055,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A131" t="s">
         <v>109</v>
       </c>
@@ -2057,7 +2063,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A132" t="s">
         <v>109</v>
       </c>
@@ -2065,7 +2071,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A133" t="s">
         <v>110</v>
       </c>
@@ -2073,7 +2079,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A134" t="s">
         <v>111</v>
       </c>
@@ -2081,7 +2087,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A135" t="s">
         <v>112</v>
       </c>
@@ -2089,7 +2095,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A136" t="s">
         <v>113</v>
       </c>
@@ -2097,7 +2103,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A137" t="s">
         <v>114</v>
       </c>
@@ -2105,7 +2111,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A138" t="s">
         <v>115</v>
       </c>
@@ -2113,7 +2119,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A139" t="s">
         <v>115</v>
       </c>
@@ -2121,7 +2127,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A140" t="s">
         <v>116</v>
       </c>
@@ -2129,7 +2135,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A141" t="s">
         <v>117</v>
       </c>
@@ -2137,7 +2143,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A142" t="s">
         <v>118</v>
       </c>
@@ -2145,7 +2151,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A143" t="s">
         <v>119</v>
       </c>
@@ -2153,7 +2159,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A144" t="s">
         <v>120</v>
       </c>
@@ -2161,7 +2167,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="145" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A145" t="s">
         <v>121</v>
       </c>
@@ -2169,7 +2175,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A146" t="s">
         <v>122</v>
       </c>
@@ -2177,7 +2183,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A147" t="s">
         <v>123</v>
       </c>
@@ -2185,7 +2191,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A148" t="s">
         <v>124</v>
       </c>
@@ -2193,7 +2199,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A149" t="s">
         <v>125</v>
       </c>
@@ -2201,7 +2207,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A150" t="s">
         <v>126</v>
       </c>
@@ -2209,7 +2215,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A151" t="s">
         <v>127</v>
       </c>
@@ -2217,7 +2223,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A152" t="s">
         <v>128</v>
       </c>
@@ -2225,7 +2231,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A153" t="s">
         <v>129</v>
       </c>
@@ -2233,7 +2239,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A154" t="s">
         <v>130</v>
       </c>
@@ -2241,7 +2247,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A155" t="s">
         <v>131</v>
       </c>
@@ -2249,7 +2255,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A156" t="s">
         <v>132</v>
       </c>
@@ -2257,7 +2263,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A157" t="s">
         <v>133</v>
       </c>
@@ -2265,7 +2271,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A158" t="s">
         <v>134</v>
       </c>
@@ -2273,7 +2279,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A159" t="s">
         <v>135</v>
       </c>
@@ -2281,7 +2287,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A160" t="s">
         <v>136</v>
       </c>
@@ -2289,7 +2295,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A161" t="s">
         <v>137</v>
       </c>
@@ -2297,7 +2303,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A162" t="s">
         <v>138</v>
       </c>
@@ -2305,7 +2311,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A163" t="s">
         <v>139</v>
       </c>
@@ -2313,7 +2319,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A164" t="s">
         <v>140</v>
       </c>
@@ -2321,7 +2327,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A165" t="s">
         <v>141</v>
       </c>
@@ -2329,7 +2335,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A166" t="s">
         <v>142</v>
       </c>
@@ -2337,7 +2343,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A167" t="s">
         <v>143</v>
       </c>
@@ -2345,7 +2351,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A168" t="s">
         <v>144</v>
       </c>
@@ -2353,7 +2359,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A169" t="s">
         <v>145</v>
       </c>
@@ -2361,7 +2367,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A170" t="s">
         <v>146</v>
       </c>
@@ -2369,7 +2375,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A171" t="s">
         <v>147</v>
       </c>
@@ -2377,7 +2383,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="172" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A172" t="s">
         <v>148</v>
       </c>
@@ -2385,7 +2391,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A173" t="s">
         <v>149</v>
       </c>
@@ -2393,7 +2399,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="174" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A174" t="s">
         <v>150</v>
       </c>
@@ -2401,7 +2407,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="175" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A175" t="s">
         <v>151</v>
       </c>
@@ -2409,7 +2415,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="176" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A176" t="s">
         <v>152</v>
       </c>
@@ -2417,7 +2423,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="177" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A177" t="s">
         <v>153</v>
       </c>
@@ -2425,7 +2431,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="178" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A178" t="s">
         <v>154</v>
       </c>
@@ -2433,7 +2439,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="179" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A179" t="s">
         <v>155</v>
       </c>
@@ -2441,7 +2447,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="180" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A180" t="s">
         <v>156</v>
       </c>
@@ -2449,7 +2455,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="181" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A181" t="s">
         <v>157</v>
       </c>
@@ -2457,7 +2463,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="182" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A182" t="s">
         <v>158</v>
       </c>
@@ -2465,7 +2471,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="183" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A183" t="s">
         <v>159</v>
       </c>
@@ -2473,7 +2479,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="184" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A184" t="s">
         <v>160</v>
       </c>
@@ -2481,7 +2487,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="185" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A185" t="s">
         <v>161</v>
       </c>
@@ -2489,7 +2495,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="186" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A186" t="s">
         <v>162</v>
       </c>
@@ -2497,7 +2503,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="187" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A187" t="s">
         <v>163</v>
       </c>
@@ -2505,7 +2511,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="188" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A188" t="s">
         <v>164</v>
       </c>
@@ -2513,7 +2519,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="189" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A189" t="s">
         <v>165</v>
       </c>
@@ -2521,7 +2527,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="190" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A190" t="s">
         <v>166</v>
       </c>
@@ -2529,7 +2535,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="191" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A191" t="s">
         <v>167</v>
       </c>
@@ -2537,7 +2543,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="192" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A192" t="s">
         <v>168</v>
       </c>
@@ -2545,7 +2551,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="193" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A193" t="s">
         <v>169</v>
       </c>
@@ -2553,7 +2559,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="194" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A194" t="s">
         <v>170</v>
       </c>
@@ -2561,7 +2567,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="195" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A195" t="s">
         <v>171</v>
       </c>
@@ -2569,7 +2575,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="196" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A196" t="s">
         <v>171</v>
       </c>
@@ -2577,7 +2583,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="197" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A197" t="s">
         <v>172</v>
       </c>
@@ -2585,7 +2591,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="198" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A198" t="s">
         <v>173</v>
       </c>
@@ -2593,7 +2599,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="199" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A199" t="s">
         <v>174</v>
       </c>
@@ -2601,7 +2607,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="200" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A200" t="s">
         <v>175</v>
       </c>
@@ -2609,7 +2615,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="201" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A201" t="s">
         <v>176</v>
       </c>
@@ -2617,7 +2623,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="202" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A202" t="s">
         <v>177</v>
       </c>
@@ -2625,7 +2631,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="203" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A203" t="s">
         <v>177</v>
       </c>
@@ -2633,7 +2639,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="204" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A204" t="s">
         <v>178</v>
       </c>
@@ -2641,7 +2647,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="205" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A205" t="s">
         <v>178</v>
       </c>
@@ -2649,7 +2655,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="206" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A206" t="s">
         <v>179</v>
       </c>
@@ -2657,7 +2663,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="207" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A207" t="s">
         <v>180</v>
       </c>
@@ -2665,7 +2671,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="208" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A208" t="s">
         <v>181</v>
       </c>
@@ -2673,7 +2679,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="209" spans="1:3" hidden="1" x14ac:dyDescent="0.45">
       <c r="A209" t="s">
         <v>182</v>
       </c>
@@ -2681,7 +2687,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="210" spans="1:3" hidden="1" x14ac:dyDescent="0.45">
       <c r="A210" t="s">
         <v>183</v>
       </c>
@@ -2689,7 +2695,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="211" spans="1:3" hidden="1" x14ac:dyDescent="0.45">
       <c r="A211" t="s">
         <v>184</v>
       </c>
@@ -2697,7 +2703,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="212" spans="1:3" hidden="1" x14ac:dyDescent="0.45">
       <c r="A212" t="s">
         <v>185</v>
       </c>
@@ -2705,7 +2711,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="213" spans="1:3" hidden="1" x14ac:dyDescent="0.45">
       <c r="A213" t="s">
         <v>186</v>
       </c>
@@ -2716,7 +2722,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="214" spans="1:3" hidden="1" x14ac:dyDescent="0.45">
       <c r="A214" t="s">
         <v>187</v>
       </c>
@@ -2724,7 +2730,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="215" spans="1:3" hidden="1" x14ac:dyDescent="0.45">
       <c r="A215" t="s">
         <v>188</v>
       </c>
@@ -2732,7 +2738,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="216" spans="1:3" hidden="1" x14ac:dyDescent="0.45">
       <c r="A216" t="s">
         <v>189</v>
       </c>
@@ -2740,7 +2746,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="217" spans="1:3" hidden="1" x14ac:dyDescent="0.45">
       <c r="A217" t="s">
         <v>190</v>
       </c>
@@ -2748,7 +2754,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="218" spans="1:3" hidden="1" x14ac:dyDescent="0.45">
       <c r="A218" t="s">
         <v>191</v>
       </c>
@@ -2756,7 +2762,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="219" spans="1:3" hidden="1" x14ac:dyDescent="0.45">
       <c r="A219" t="s">
         <v>192</v>
       </c>
@@ -2764,7 +2770,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="220" spans="1:3" hidden="1" x14ac:dyDescent="0.45">
       <c r="A220" t="s">
         <v>193</v>
       </c>
@@ -2772,7 +2778,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="221" spans="1:3" hidden="1" x14ac:dyDescent="0.45">
       <c r="A221" t="s">
         <v>194</v>
       </c>
@@ -2780,7 +2786,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="222" spans="1:3" hidden="1" x14ac:dyDescent="0.45">
       <c r="A222" t="s">
         <v>195</v>
       </c>
@@ -2788,7 +2794,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="223" spans="1:3" hidden="1" x14ac:dyDescent="0.45">
       <c r="A223" t="s">
         <v>196</v>
       </c>
@@ -2796,7 +2802,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="224" spans="1:3" hidden="1" x14ac:dyDescent="0.45">
       <c r="A224" t="s">
         <v>197</v>
       </c>
@@ -2804,7 +2810,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="225" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A225" t="s">
         <v>198</v>
       </c>
@@ -2812,7 +2818,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="226" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A226" t="s">
         <v>199</v>
       </c>
@@ -2820,7 +2826,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="227" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A227" t="s">
         <v>200</v>
       </c>
@@ -2832,7 +2838,7 @@
   <autoFilter ref="A1:C227">
     <filterColumn colId="1">
       <filters>
-        <filter val="Передняя левая центральная (мм)"/>
+        <filter val="Без мотора"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>